<commit_message>
added cheshire honey pot glen
</commit_message>
<xml_diff>
--- a/otl-covenants-tables.xlsx
+++ b/otl-covenants-tables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="318">
   <si>
     <t>id</t>
   </si>
@@ -57,6 +57,33 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>cheshire_honey_pot_glen</t>
+  </si>
+  <si>
+    <t>Cheshire</t>
+  </si>
+  <si>
+    <t>Honey Pot Glen</t>
+  </si>
+  <si>
+    <t>subdivision</t>
+  </si>
+  <si>
+    <t>Country Club Rd, Glen Ct, Glenbrook Dr, Wolf Hill Rd</t>
+  </si>
+  <si>
+    <t>counted addresses linked to restricted lots in spreadsheet</t>
+  </si>
+  <si>
+    <t>vol. 62, pp. 299-232, with maps</t>
+  </si>
+  <si>
+    <t>August Anderson</t>
+  </si>
+  <si>
+    <t>No persons of any race other than the white race shall use or occupy any building on any lot except that this covenant shall not prevent the occupancy by domestic servants of a different race domiciled with an owner or tenant.</t>
+  </si>
+  <si>
     <t>easthaddam_lake_hayward_club</t>
   </si>
   <si>
@@ -66,9 +93,6 @@
     <t>Lake Hayward Club</t>
   </si>
   <si>
-    <t>subdivision</t>
-  </si>
-  <si>
     <t>Briarcliff Rd, Cragmere Rd, East Lane, Forest Way, Glimmer Glen, Hay Field Rd, Hillside Rd, Lake Hayward Town Rd, Lake Shore Dr, Laurel Lane, Longwood Dr, Lookout Dr, Ridgewood Dr, Ridgewood Dr Ext, Sunset Rd, Wildwood Rd</t>
   </si>
   <si>
@@ -96,12 +120,15 @@
     <t>although 624 original lots, 79 properties with addresses listed on roads by Town Assessor</t>
   </si>
   <si>
-    <t>vol. 68, p. 30, with town maps</t>
+    <t>vol. 68, p. 30; vol 63, p. 103, with town maps</t>
   </si>
   <si>
     <t>Edward L. Parker and Curtis L. Jones, The Lake Realty Company</t>
   </si>
   <si>
+    <t>20 October 1947; 21 December 1950</t>
+  </si>
+  <si>
     <t>No portion of said premises shall be conveyed or leased to any other than the Caucasian Race.</t>
   </si>
   <si>
@@ -235,9 +262,6 @@
   </si>
   <si>
     <t>Joseph E. Maselli and Pasquale DeRosa</t>
-  </si>
-  <si>
-    <t>No persons of any race other than the white race shall use or occupy any building on any lot except that this covenant shall not prevent the occupancy by domestic servants of a different race domiciled with an owner or tenant.</t>
   </si>
   <si>
     <t>hamden_northside</t>
@@ -564,7 +588,46 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>otl-covenants-tables by Jack Dougherty for OnTheLine.trincoll.edu</t>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">otl-covenants-tables by Jack Dougherty, June Gold, David Ware for </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>myCTdeed.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>OnTheLine.trincoll.edu</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated percent of homes with racial covenants among all homes (or buildings) built during period </t>
+  </si>
+  <si>
+    <t xml:space="preserve">see hamden-calc </t>
+  </si>
+  <si>
+    <t>see westhartford-calc</t>
+  </si>
+  <si>
+    <t>of homes built 1910-1950 (Ware 2020, p. 15)</t>
   </si>
   <si>
     <t>How to update: scan historical docs, draw in GeoJson.io, data entry in Google Sheet, join in MapShaper, republish in Datawrapper, save to GitHub</t>
@@ -597,7 +660,7 @@
     </r>
   </si>
   <si>
-    <t>to enter new data, go to data in Google Sheet; avoid empty rows at bottom for cleaner pivot table</t>
+    <t>to enter new data, go to data in Google Sheet; avoid empty rows at bottom for cleaner pivot table (*but ensure that pivot table reads all rows!)</t>
   </si>
   <si>
     <t>download data as CSV</t>
@@ -662,24 +725,6 @@
     <t>https://ontheline.trincoll.edu/restricting.html</t>
   </si>
   <si>
-    <t xml:space="preserve">Estimated percent of homes with racial covenants among all homes or building built during period </t>
-  </si>
-  <si>
-    <t>Estimated percent of all homes built in 1940s</t>
-  </si>
-  <si>
-    <t>TBA</t>
-  </si>
-  <si>
-    <t>22% of homes built during 1940s, based on HamdenParcels file from Andrew Kinlock, Town of Hamden GIS coordinator, Feb 2024</t>
-  </si>
-  <si>
-    <t>3.5% of homes built 1910-1950 (Ware 2020)</t>
-  </si>
-  <si>
-    <t>6% of buildings built during 1940s</t>
-  </si>
-  <si>
     <t>Sources</t>
   </si>
   <si>
@@ -999,10 +1044,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d&quot; &quot;mmmm&quot; &quot;yyyy"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -1021,6 +1067,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11.0"/>
+      <color rgb="FF0000FF"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -1031,6 +1082,12 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -1101,7 +1158,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1119,26 +1176,27 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1153,25 +1211,31 @@
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="9" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="9" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="9" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1207,11 +1271,12 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" invalid="1" refreshOnLoad="1">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:Z27" sheet="data"/>
+    <worksheetSource ref="A1:Z28" sheet="data"/>
   </cacheSource>
   <cacheFields>
     <cacheField name="id" numFmtId="0">
       <sharedItems>
+        <s v="cheshire_honey_pot_glen"/>
         <s v="easthaddam_lake_hayward_club"/>
         <s v="easthaddam_moodus_estates"/>
         <s v="easthaddam_moodus_lake_shores"/>
@@ -1242,6 +1307,7 @@
     </cacheField>
     <cacheField name="town" numFmtId="0">
       <sharedItems>
+        <s v="Cheshire"/>
         <s v="East Haddam"/>
         <s v="Hamden"/>
         <s v="Manchester"/>
@@ -1252,6 +1318,7 @@
     </cacheField>
     <cacheField name="name" numFmtId="0">
       <sharedItems>
+        <s v="Honey Pot Glen"/>
         <s v="Lake Hayward Club"/>
         <s v="Moodus Estates"/>
         <s v="Moodus Lake Shores"/>
@@ -1287,6 +1354,7 @@
     </cacheField>
     <cacheField name="streets-partial" numFmtId="0">
       <sharedItems>
+        <s v="Country Club Rd, Glen Ct, Glenbrook Dr, Wolf Hill Rd"/>
         <s v="Briarcliff Rd, Cragmere Rd, East Lane, Forest Way, Glimmer Glen, Hay Field Rd, Hillside Rd, Lake Hayward Town Rd, Lake Shore Dr, Laurel Lane, Longwood Dr, Lookout Dr, Ridgewood Dr, Ridgewood Dr Ext, Sunset Rd, Wildwood Rd"/>
         <s v="Laurel Rd, White Sands Road, Pine Tree Rd, Birch Road, Woodland Rd, Lakeview Rd. Shore Dr, Sands Rd, Crestview Road, Hill Top Road"/>
         <s v="Beach Rd, Berry Rd, Birch Rd, Britain Rd, Camp Rd, Emily Rd, Geronimo Rd, Grama Rd, Hilltop Rd, Mabel Rd, Maple Rd, Oak Rd, Paula Rd, Pine Rd, Rock Rd, Shady Rd, Short Rd, Steven Rd, Swamp Rd, Tom Rd, Ward Rd"/>
@@ -1317,6 +1385,7 @@
     </cacheField>
     <cacheField name="est-homes" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1">
+        <n v="43.0"/>
         <n v="418.0"/>
         <n v="79.0"/>
         <n v="75.0"/>
@@ -1346,6 +1415,7 @@
     </cacheField>
     <cacheField name="est-notes" numFmtId="0">
       <sharedItems>
+        <s v="counted addresses linked to restricted lots in spreadsheet"/>
         <s v="although 750 original lots, 418 properties with addresses listed on roads by Town Assessor"/>
         <s v="although 624 original lots, 79 properties with addresses listed on roads by Town Assessor"/>
         <s v="although 407 original lots, 75 properties with addresses listed on roads by Town Assessor"/>
@@ -1361,8 +1431,9 @@
     </cacheField>
     <cacheField name="source" numFmtId="0">
       <sharedItems>
+        <s v="vol. 62, pp. 299-232, with maps"/>
         <s v="vol. 56, p. 111, with town maps"/>
-        <s v="vol. 68, p. 30, with town maps"/>
+        <s v="vol. 68, p. 30; vol 63, p. 103, with town maps"/>
         <s v="vol. 61, p. 392, with town maps"/>
         <s v="vol. 63, p. 538, with town maps"/>
         <s v="vol. 199, pp. 589-90, and map 152a"/>
@@ -1391,6 +1462,7 @@
     </cacheField>
     <cacheField name="restrictor" numFmtId="0">
       <sharedItems>
+        <s v="August Anderson"/>
         <s v="James Jay Smith, President of The Shore &amp; Lake Corp."/>
         <s v="Edward L. Parker and Curtis L. Jones, The Lake Realty Company"/>
         <s v="Edward L. Parker and Curtis L. Jones, The Lakeshore Company"/>
@@ -1418,10 +1490,11 @@
         <s v="Martin Lohne, Secretary of The Berner Lohne Company"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="date" numFmtId="164">
-      <sharedItems containsSemiMixedTypes="0" containsDate="1" containsString="0">
+    <cacheField name="date">
+      <sharedItems containsDate="1" containsMixedTypes="1">
+        <d v="1940-11-14T00:00:00Z"/>
         <d v="1936-07-10T00:00:00Z"/>
-        <d v="1947-10-20T00:00:00Z"/>
+        <s v="20 October 1947; 21 December 1950"/>
         <d v="1946-11-21T00:00:00Z"/>
         <d v="1948-08-28T00:00:00Z"/>
         <d v="1940-01-02T00:00:00Z"/>
@@ -1450,6 +1523,7 @@
     </cacheField>
     <cacheField name="text" numFmtId="0">
       <sharedItems>
+        <s v="No persons of any race other than the white race shall use or occupy any building on any lot except that this covenant shall not prevent the occupancy by domestic servants of a different race domiciled with an owner or tenant."/>
         <s v="As the Lake Hayward Club property is strictly a club proposition, it is hereby covenants and agreed that the property herein conveyed shall not be sold, released, or rented in any form or manner directly or indirectly to any person or persons: (1) who are"/>
         <s v="No portion of said premises shall be conveyed or leased to any other than the Caucasian Race."/>
         <s v="The use and occupancy of said premises shall be limited to the use of members of the Caucasian Race, except for domestic servants."/>
@@ -1457,7 +1531,6 @@
         <s v="No persons of any race other than the white race shall use or occupy any building or any lot, except that this covenant shall not prevent occupancy by domestic servants of a different race domiciled with an owner or tenant."/>
         <s v="No person of any race other than the white race shall use or occupy any building or any lot, except that this covenant shall not prevent the occupancy by domestic servants of a different race domiciled with an owner or tenant of any building."/>
         <s v="No persons of any race other than the white race shall use or occupy any building or any lot except that this covenant shall not prevent the occupant by domestic servants of a different race domiciled with an owner or tenant."/>
-        <s v="No persons of any race other than the white race shall use or occupy any building on any lot except that this covenant shall not prevent the occupancy by domestic servants of a different race domiciled with an owner or tenant."/>
         <s v="No persons of any race other than the white race shall use or occupy any building or any lot, except that this covenant shall not prevent the occupancy by domestic servants of a different race domiciled with an owner or tenant."/>
         <s v="No persons of any race other than the white race, shall use or occupy any building or any lot, except that this covenant shall not prevent occupancy by domestic servants of a different race, domiciled with an owner or tenant."/>
         <s v="No persons of any race other than the white race shall use or occupy any building or any lot except that this covenant shall not prevent the occupancy by domestic servants of a different race domiciled with an owner or tenant."/>
@@ -1551,7 +1624,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="pivot" cacheId="0" dataCaption="" compact="0" compactData="0">
-  <location ref="A1:C8" firstHeaderRow="0" firstDataRow="2" firstDataCol="0"/>
+  <location ref="A1:C9" firstHeaderRow="0" firstDataRow="2" firstDataCol="0"/>
   <pivotFields>
     <pivotField name="id" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items>
@@ -1581,6 +1654,7 @@
         <item x="23"/>
         <item x="24"/>
         <item x="25"/>
+        <item x="26"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1592,6 +1666,7 @@
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1623,6 +1698,7 @@
         <item x="23"/>
         <item x="24"/>
         <item x="25"/>
+        <item x="26"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1660,6 +1736,7 @@
         <item x="23"/>
         <item x="24"/>
         <item x="25"/>
+        <item x="26"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1690,6 +1767,7 @@
         <item x="22"/>
         <item x="23"/>
         <item x="24"/>
+        <item x="25"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1706,6 +1784,7 @@
         <item x="8"/>
         <item x="9"/>
         <item x="10"/>
+        <item x="11"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1737,6 +1816,7 @@
         <item x="23"/>
         <item x="24"/>
         <item x="25"/>
+        <item x="26"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1767,10 +1847,11 @@
         <item x="22"/>
         <item x="23"/>
         <item x="24"/>
+        <item x="25"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField name="date" compact="0" numFmtId="164" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+    <pivotField name="date" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items>
         <item x="0"/>
         <item x="1"/>
@@ -1798,6 +1879,7 @@
         <item x="23"/>
         <item x="24"/>
         <item x="25"/>
+        <item x="26"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2138,7 +2220,9 @@
     <col customWidth="1" min="4" max="4" width="9.1"/>
     <col customWidth="1" min="5" max="5" width="18.7"/>
     <col customWidth="1" min="6" max="7" width="11.2"/>
-    <col customWidth="1" min="8" max="26" width="18.7"/>
+    <col customWidth="1" min="8" max="8" width="18.7"/>
+    <col customWidth="1" min="9" max="9" width="29.2"/>
+    <col customWidth="1" min="10" max="26" width="18.7"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
@@ -2238,7 +2322,7 @@
         <v>16</v>
       </c>
       <c r="F2" s="4">
-        <v>418.0</v>
+        <v>43.0</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>17</v>
@@ -2250,7 +2334,7 @@
         <v>19</v>
       </c>
       <c r="J2" s="5">
-        <v>13341.0</v>
+        <v>14929.0</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>20</v>
@@ -2276,34 +2360,34 @@
         <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F3" s="4">
-        <v>79.0</v>
+        <v>418.0</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J3" s="5">
-        <v>17460.0</v>
+        <v>13341.0</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -2323,37 +2407,37 @@
     </row>
     <row r="4" ht="15.0" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F4" s="4">
-        <v>75.0</v>
+        <v>79.0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" s="5">
-        <v>17127.0</v>
+        <v>34</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -2373,37 +2457,37 @@
     </row>
     <row r="5" ht="15.0" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="4">
+        <v>75.0</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="5">
+        <v>17127.0</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="F5" s="4">
-        <v>32.0</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="5">
-        <v>17773.0</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -2422,38 +2506,38 @@
       <c r="Z5" s="3"/>
     </row>
     <row r="6" ht="15.0" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="F6" s="4">
+        <v>32.0</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="2">
-        <v>14612.0</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="H6" s="4" t="s">
         <v>47</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="5">
+        <v>17773.0</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -2473,37 +2557,37 @@
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F7" s="1">
-        <v>28.0</v>
+        <v>11.0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="J7" s="2">
-        <v>15512.0</v>
+        <v>14612.0</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -2523,37 +2607,37 @@
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F8" s="1">
-        <v>20.0</v>
+        <v>28.0</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J8" s="2">
-        <v>15465.0</v>
+        <v>15512.0</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -2573,37 +2657,37 @@
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F9" s="1">
-        <v>49.0</v>
+        <v>20.0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J9" s="2">
-        <v>15235.0</v>
+        <v>15465.0</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -2623,37 +2707,37 @@
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="4">
-        <v>81.0</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="F10" s="1">
+        <v>49.0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J10" s="2">
-        <v>14885.0</v>
+        <v>15235.0</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -2673,37 +2757,37 @@
     </row>
     <row r="11" ht="15.0" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="1">
-        <v>53.0</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
+      </c>
+      <c r="F11" s="4">
+        <v>81.0</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J11" s="2">
-        <v>16782.0</v>
+        <v>14885.0</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
@@ -2723,37 +2807,37 @@
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F12" s="1">
-        <v>44.0</v>
+        <v>53.0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J12" s="2">
-        <v>14916.0</v>
+        <v>16782.0</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -2773,37 +2857,37 @@
     </row>
     <row r="13" ht="15.0" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F13" s="1">
-        <v>89.0</v>
+        <v>44.0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J13" s="2">
-        <v>14713.0</v>
+        <v>14916.0</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -2823,37 +2907,37 @@
     </row>
     <row r="14" ht="15.0" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F14" s="1">
-        <v>25.0</v>
+        <v>89.0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J14" s="2">
-        <v>15326.0</v>
+        <v>14713.0</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -2873,37 +2957,37 @@
     </row>
     <row r="15" ht="15.0" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F15" s="1">
-        <v>47.0</v>
+        <v>25.0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J15" s="2">
-        <v>15250.0</v>
+        <v>15326.0</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
@@ -2923,37 +3007,37 @@
     </row>
     <row r="16" ht="15.0" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F16" s="1">
-        <v>74.0</v>
+        <v>47.0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="J16" s="2">
-        <v>14731.0</v>
+        <v>15250.0</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -2973,37 +3057,37 @@
     </row>
     <row r="17" ht="15.0" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F17" s="3">
-        <v>104.0</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>44</v>
+        <v>113</v>
+      </c>
+      <c r="F17" s="1">
+        <v>74.0</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="J17" s="2">
-        <v>14734.0</v>
+        <v>14731.0</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -3023,37 +3107,37 @@
     </row>
     <row r="18" ht="15.0" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F18" s="3">
-        <v>118.0</v>
+        <v>104.0</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J18" s="2">
-        <v>14933.0</v>
+        <v>14734.0</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -3073,37 +3157,37 @@
     </row>
     <row r="19" ht="15.0" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F19" s="3">
-        <v>18.0</v>
+        <v>118.0</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="J19" s="2">
-        <v>15148.0</v>
+        <v>14933.0</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
@@ -3123,37 +3207,37 @@
     </row>
     <row r="20" ht="15.0" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F20" s="3">
-        <v>47.0</v>
+        <v>18.0</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="J20" s="2">
-        <v>14522.0</v>
+        <v>15148.0</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>130</v>
+        <v>62</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -3173,37 +3257,37 @@
     </row>
     <row r="21" ht="15.0" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F21" s="3">
-        <v>26.0</v>
+        <v>47.0</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J21" s="2">
-        <v>14599.0</v>
+        <v>14522.0</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -3223,25 +3307,25 @@
     </row>
     <row r="22" ht="15.0" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F22" s="6">
-        <v>12.0</v>
-      </c>
-      <c r="G22" s="6" t="s">
         <v>141</v>
+      </c>
+      <c r="F22" s="3">
+        <v>26.0</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>142</v>
@@ -3250,7 +3334,7 @@
         <v>143</v>
       </c>
       <c r="J22" s="2">
-        <v>14914.0</v>
+        <v>14599.0</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>144</v>
@@ -3276,34 +3360,34 @@
         <v>145</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F23" s="6">
-        <v>19.0</v>
+        <v>12.0</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J23" s="2">
-        <v>15186.0</v>
+        <v>14914.0</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -3323,37 +3407,37 @@
     </row>
     <row r="24" ht="15.0" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F24" s="6">
-        <v>84.0</v>
+        <v>19.0</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J24" s="2">
-        <v>14772.0</v>
+        <v>15186.0</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
@@ -3373,37 +3457,37 @@
     </row>
     <row r="25" ht="15.0" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F25" s="6">
-        <v>41.0</v>
+        <v>84.0</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J25" s="2">
-        <v>15122.0</v>
+        <v>14772.0</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
@@ -3423,37 +3507,37 @@
     </row>
     <row r="26" ht="15.0" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F26" s="6">
-        <v>34.0</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>165</v>
+        <v>41.0</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="J26" s="2">
-        <v>14779.0</v>
+        <v>15122.0</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
@@ -3472,37 +3556,37 @@
       <c r="Z26" s="3"/>
     </row>
     <row r="27" ht="15.0" customHeight="1">
-      <c r="A27" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B27" s="4" t="s">
+      <c r="A27" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="F27" s="4">
-        <v>35.0</v>
+      <c r="F27" s="6">
+        <v>34.0</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="J27" s="5">
-        <v>14626.0</v>
-      </c>
-      <c r="K27" s="4" t="s">
+      <c r="J27" s="2">
+        <v>14779.0</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>176</v>
       </c>
       <c r="L27" s="3"/>
@@ -3520,6 +3604,56 @@
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
+    </row>
+    <row r="28" ht="15.0" customHeight="1">
+      <c r="A28" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="F28" s="4">
+        <v>35.0</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="J28" s="5">
+        <v>14626.0</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
     </row>
   </sheetData>
   <printOptions/>
@@ -3547,6 +3681,7 @@
     <row r="6"/>
     <row r="7"/>
     <row r="8"/>
+    <row r="9"/>
   </sheetData>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -3564,7 +3699,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -3620,130 +3755,48 @@
       <c r="Y2" s="9"/>
       <c r="Z2" s="9"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9"/>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9"/>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
+    <row r="3">
+      <c r="A3" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="12">
+        <f>'hamden-calc'!B16</f>
+        <v>0.2268175882</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="12">
+        <f>'westhartford-calc'!B16</f>
+        <v>0.06291390728</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="14">
+        <v>0.035</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="13" t="s">
-        <v>185</v>
-      </c>
+      <c r="A7" s="10"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -3771,8 +3824,8 @@
       <c r="Z7" s="9"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="12" t="s">
-        <v>186</v>
+      <c r="A8" s="10" t="s">
+        <v>193</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -3801,8 +3854,8 @@
       <c r="Z8" s="9"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="13" t="s">
-        <v>187</v>
+      <c r="A9" s="16" t="s">
+        <v>194</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -3831,8 +3884,8 @@
       <c r="Z9" s="9"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="13" t="s">
-        <v>188</v>
+      <c r="A10" s="17" t="s">
+        <v>195</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -3861,8 +3914,8 @@
       <c r="Z10" s="9"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="13" t="s">
-        <v>189</v>
+      <c r="A11" s="15" t="s">
+        <v>196</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -3891,8 +3944,8 @@
       <c r="Z11" s="9"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="13" t="s">
-        <v>190</v>
+      <c r="A12" s="15" t="s">
+        <v>197</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -3921,8 +3974,8 @@
       <c r="Z12" s="9"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="11" t="s">
-        <v>191</v>
+      <c r="A13" s="17" t="s">
+        <v>198</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -3951,8 +4004,8 @@
       <c r="Z13" s="9"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="13" t="s">
-        <v>192</v>
+      <c r="A14" s="15" t="s">
+        <v>199</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -3981,108 +4034,209 @@
       <c r="Z14" s="9"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="14" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="A15" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>194</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="14" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="18">
+      <c r="A17" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="16" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="17" t="s">
-        <v>198</v>
+        <v>203</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="13" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="14" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="16" t="s">
-        <v>200</v>
+      <c r="A21" s="18" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="13" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="14"/>
+      <c r="A23" s="19" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="14" t="s">
-        <v>201</v>
+      <c r="A24" s="13" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="25">
-      <c r="B25" s="7" t="s">
-        <v>202</v>
+      <c r="A25" s="20" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>203</v>
+      <c r="A26" s="13" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>204</v>
+      <c r="A27" s="19" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>203</v>
-      </c>
+      <c r="A28" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A5"/>
-    <hyperlink r:id="rId2" ref="A8"/>
-    <hyperlink r:id="rId3" location="/dCnch" ref="A16"/>
-    <hyperlink r:id="rId4" location="/j4lCy" ref="A18"/>
-    <hyperlink r:id="rId5" ref="A20"/>
-    <hyperlink r:id="rId6" ref="A22"/>
+    <hyperlink r:id="rId1" ref="A1"/>
+    <hyperlink r:id="rId2" ref="A10"/>
+    <hyperlink r:id="rId3" ref="A13"/>
+    <hyperlink r:id="rId4" location="/dCnch" ref="A21"/>
+    <hyperlink r:id="rId5" location="/j4lCy" ref="A23"/>
+    <hyperlink r:id="rId6" ref="A25"/>
+    <hyperlink r:id="rId7" ref="A27"/>
   </hyperlinks>
-  <drawing r:id="rId7"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -4102,70 +4256,70 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="Q1" s="18"/>
+      <c r="A1" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q1" s="21"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q2" s="18"/>
+      <c r="A2" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q2" s="21"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q3" s="18"/>
+      <c r="A3" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q3" s="21"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q4" s="18"/>
+      <c r="A4" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q4" s="21"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q5" s="18"/>
+      <c r="A5" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q5" s="21"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q6" s="18"/>
+      <c r="A6" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q6" s="21"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q7" s="18"/>
+      <c r="A7" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q7" s="21"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q8" s="18"/>
+      <c r="A8" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q8" s="21"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q9" s="18"/>
+      <c r="A9" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q9" s="21"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="Q10" s="18"/>
+      <c r="A10" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q10" s="21"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q11" s="18"/>
+      <c r="A11" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q11" s="21"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
@@ -4179,11 +4333,11 @@
       <c r="I12" s="1"/>
       <c r="J12" s="2"/>
       <c r="K12" s="1"/>
-      <c r="Q12" s="18"/>
+      <c r="Q12" s="21"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -4195,11 +4349,11 @@
       <c r="I13" s="1"/>
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
-      <c r="Q13" s="18"/>
+      <c r="Q13" s="21"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -4211,11 +4365,11 @@
       <c r="I14" s="1"/>
       <c r="J14" s="2"/>
       <c r="K14" s="1"/>
-      <c r="Q14" s="18"/>
+      <c r="Q14" s="21"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -4227,11 +4381,11 @@
       <c r="I15" s="1"/>
       <c r="J15" s="2"/>
       <c r="K15" s="1"/>
-      <c r="Q15" s="18"/>
+      <c r="Q15" s="21"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -4243,11 +4397,11 @@
       <c r="I16" s="1"/>
       <c r="J16" s="2"/>
       <c r="K16" s="1"/>
-      <c r="Q16" s="18"/>
+      <c r="Q16" s="21"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -4259,11 +4413,11 @@
       <c r="I17" s="1"/>
       <c r="J17" s="2"/>
       <c r="K17" s="1"/>
-      <c r="Q17" s="18"/>
+      <c r="Q17" s="21"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -4275,11 +4429,11 @@
       <c r="I18" s="1"/>
       <c r="J18" s="2"/>
       <c r="K18" s="1"/>
-      <c r="Q18" s="18"/>
+      <c r="Q18" s="21"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -4291,11 +4445,11 @@
       <c r="I19" s="1"/>
       <c r="J19" s="2"/>
       <c r="K19" s="1"/>
-      <c r="Q19" s="18"/>
+      <c r="Q19" s="21"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="19" t="s">
-        <v>225</v>
+      <c r="A20" s="22" t="s">
+        <v>231</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -4307,11 +4461,11 @@
       <c r="I20" s="1"/>
       <c r="J20" s="2"/>
       <c r="K20" s="1"/>
-      <c r="Q20" s="18"/>
+      <c r="Q20" s="21"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -4323,11 +4477,11 @@
       <c r="I21" s="1"/>
       <c r="J21" s="2"/>
       <c r="K21" s="1"/>
-      <c r="Q21" s="18"/>
+      <c r="Q21" s="21"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="20" t="s">
-        <v>227</v>
+      <c r="A22" s="23" t="s">
+        <v>233</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -4339,11 +4493,11 @@
       <c r="I22" s="1"/>
       <c r="J22" s="2"/>
       <c r="K22" s="1"/>
-      <c r="Q22" s="18"/>
+      <c r="Q22" s="21"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -4355,11 +4509,11 @@
       <c r="I23" s="1"/>
       <c r="J23" s="2"/>
       <c r="K23" s="1"/>
-      <c r="Q23" s="18"/>
+      <c r="Q23" s="21"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="19" t="s">
-        <v>229</v>
+      <c r="A24" s="22" t="s">
+        <v>235</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -4371,11 +4525,11 @@
       <c r="I24" s="1"/>
       <c r="J24" s="2"/>
       <c r="K24" s="1"/>
-      <c r="Q24" s="18"/>
+      <c r="Q24" s="21"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -4387,11 +4541,11 @@
       <c r="I25" s="1"/>
       <c r="J25" s="2"/>
       <c r="K25" s="1"/>
-      <c r="Q25" s="18"/>
+      <c r="Q25" s="21"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -4403,11 +4557,11 @@
       <c r="I26" s="1"/>
       <c r="J26" s="2"/>
       <c r="K26" s="1"/>
-      <c r="Q26" s="18"/>
+      <c r="Q26" s="21"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="19" t="s">
-        <v>232</v>
+      <c r="A27" s="22" t="s">
+        <v>238</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -4419,11 +4573,11 @@
       <c r="I27" s="1"/>
       <c r="J27" s="2"/>
       <c r="K27" s="1"/>
-      <c r="Q27" s="18"/>
+      <c r="Q27" s="21"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -4435,11 +4589,11 @@
       <c r="I28" s="1"/>
       <c r="J28" s="2"/>
       <c r="K28" s="1"/>
-      <c r="Q28" s="18"/>
+      <c r="Q28" s="21"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="19" t="s">
-        <v>234</v>
+      <c r="A29" s="22" t="s">
+        <v>240</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -4451,11 +4605,11 @@
       <c r="I29" s="1"/>
       <c r="J29" s="2"/>
       <c r="K29" s="1"/>
-      <c r="Q29" s="18"/>
+      <c r="Q29" s="21"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="19" t="s">
-        <v>235</v>
+      <c r="A30" s="22" t="s">
+        <v>241</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -4467,7 +4621,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="2"/>
       <c r="K30" s="1"/>
-      <c r="Q30" s="18"/>
+      <c r="Q30" s="21"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1"/>
@@ -4481,7 +4635,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="2"/>
       <c r="K31" s="1"/>
-      <c r="Q31" s="18"/>
+      <c r="Q31" s="21"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
@@ -4517,17 +4671,17 @@
       <c r="K32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Q32" s="18"/>
+      <c r="Q32" s="21"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>15</v>
@@ -4535,679 +4689,679 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="J33" s="5">
         <v>18396.0</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q33" s="18"/>
+        <v>247</v>
+      </c>
+      <c r="Q33" s="21"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="Q34" s="18"/>
+      <c r="Q34" s="21"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q35" s="18"/>
+      <c r="A35" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q35" s="21"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="B36" s="14">
+      <c r="A36" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="B36" s="13">
         <v>10.0</v>
       </c>
-      <c r="Q36" s="18"/>
+      <c r="Q36" s="21"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="B37" s="14">
+      <c r="A37" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="B37" s="13">
         <v>12.0</v>
       </c>
-      <c r="Q37" s="18"/>
+      <c r="Q37" s="21"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="B38" s="14">
+      <c r="A38" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="B38" s="13">
         <v>4.0</v>
       </c>
-      <c r="Q38" s="18"/>
+      <c r="Q38" s="21"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="B39" s="14">
+      <c r="A39" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="B39" s="13">
         <v>22.0</v>
       </c>
-      <c r="Q39" s="18"/>
+      <c r="Q39" s="21"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="B40" s="14">
+      <c r="A40" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B40" s="13">
         <v>28.0</v>
       </c>
-      <c r="Q40" s="18"/>
+      <c r="Q40" s="21"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="B41" s="14">
+      <c r="A41" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="B41" s="13">
         <v>13.0</v>
       </c>
-      <c r="Q41" s="18"/>
+      <c r="Q41" s="21"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="B42" s="14">
+      <c r="A42" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B42" s="13">
         <v>4.0</v>
       </c>
-      <c r="Q42" s="18"/>
+      <c r="Q42" s="21"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="B43" s="14">
+      <c r="A43" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="B43" s="13">
         <v>11.0</v>
       </c>
-      <c r="Q43" s="18"/>
+      <c r="Q43" s="21"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="B44" s="14">
+      <c r="A44" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="B44" s="13">
         <v>105.0</v>
       </c>
-      <c r="Q44" s="18"/>
+      <c r="Q44" s="21"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="B45" s="14">
+      <c r="A45" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="B45" s="13">
         <v>5.0</v>
       </c>
-      <c r="Q45" s="18"/>
+      <c r="Q45" s="21"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="B46" s="14">
+      <c r="A46" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="B46" s="13">
         <v>54.0</v>
       </c>
-      <c r="Q46" s="18"/>
+      <c r="Q46" s="21"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="B47" s="14">
+      <c r="A47" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="B47" s="13">
         <v>32.0</v>
       </c>
-      <c r="Q47" s="18"/>
+      <c r="Q47" s="21"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="B48" s="14">
+      <c r="A48" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="B48" s="13">
         <v>40.0</v>
       </c>
-      <c r="Q48" s="18"/>
+      <c r="Q48" s="21"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="B49" s="14">
+      <c r="A49" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="B49" s="13">
         <v>10.0</v>
       </c>
-      <c r="Q49" s="18"/>
+      <c r="Q49" s="21"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="B50" s="14">
+      <c r="A50" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="B50" s="13">
         <v>8.0</v>
       </c>
-      <c r="Q50" s="18"/>
+      <c r="Q50" s="21"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="B51" s="14">
+      <c r="A51" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="B51" s="13">
         <v>60.0</v>
       </c>
-      <c r="Q51" s="18"/>
+      <c r="Q51" s="21"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="14" t="s">
-        <v>259</v>
+      <c r="A52" s="13" t="s">
+        <v>265</v>
       </c>
       <c r="B52" s="7">
         <f>sum(B36:B51)</f>
         <v>418</v>
       </c>
-      <c r="Q52" s="18"/>
+      <c r="Q52" s="21"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="Q53" s="18"/>
+      <c r="Q53" s="21"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="Q54" s="18"/>
+      <c r="Q54" s="21"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B55" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q55" s="18"/>
+      <c r="A55" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q55" s="21"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="21" t="s">
-        <v>260</v>
-      </c>
-      <c r="B56" s="14">
+      <c r="A56" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="B56" s="13">
         <v>9.0</v>
       </c>
-      <c r="Q56" s="18"/>
+      <c r="Q56" s="21"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="21" t="s">
-        <v>261</v>
-      </c>
-      <c r="B57" s="14">
+      <c r="A57" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="B57" s="13">
         <v>4.0</v>
       </c>
-      <c r="Q57" s="18"/>
+      <c r="Q57" s="21"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="B58" s="14">
+      <c r="A58" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="B58" s="13">
         <v>8.0</v>
       </c>
-      <c r="Q58" s="18"/>
+      <c r="Q58" s="21"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="21" t="s">
-        <v>263</v>
-      </c>
-      <c r="B59" s="14">
+      <c r="A59" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="B59" s="13">
         <v>2.0</v>
       </c>
-      <c r="Q59" s="18"/>
+      <c r="Q59" s="21"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="21" t="s">
-        <v>264</v>
-      </c>
-      <c r="B60" s="14">
+      <c r="A60" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="B60" s="13">
         <v>6.0</v>
       </c>
-      <c r="Q60" s="18"/>
+      <c r="Q60" s="21"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="21" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q61" s="18"/>
+      <c r="A61" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q61" s="21"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="21" t="s">
-        <v>266</v>
-      </c>
-      <c r="B62" s="14">
+      <c r="A62" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="B62" s="13">
         <v>5.0</v>
       </c>
-      <c r="Q62" s="18"/>
+      <c r="Q62" s="21"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="21" t="s">
-        <v>267</v>
-      </c>
-      <c r="B63" s="14">
+      <c r="A63" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="B63" s="13">
         <v>1.0</v>
       </c>
-      <c r="Q63" s="18"/>
+      <c r="Q63" s="21"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="B64" s="14">
+      <c r="A64" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="B64" s="13">
         <v>16.0</v>
       </c>
-      <c r="Q64" s="18"/>
+      <c r="Q64" s="21"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="21" t="s">
-        <v>269</v>
-      </c>
-      <c r="B65" s="14">
+      <c r="A65" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="B65" s="13">
         <v>11.0</v>
       </c>
-      <c r="Q65" s="18"/>
+      <c r="Q65" s="21"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="21" t="s">
-        <v>270</v>
-      </c>
-      <c r="B66" s="14">
+      <c r="A66" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="B66" s="13">
         <v>11.0</v>
       </c>
-      <c r="Q66" s="18"/>
+      <c r="Q66" s="21"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="B67" s="14">
+      <c r="A67" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="B67" s="13">
         <v>6.0</v>
       </c>
-      <c r="Q67" s="18"/>
+      <c r="Q67" s="21"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="Q68" s="18"/>
+      <c r="A68" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q68" s="21"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="14" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q69" s="18"/>
+      <c r="A69" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q69" s="21"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="14" t="s">
-        <v>274</v>
+      <c r="A70" s="13" t="s">
+        <v>280</v>
       </c>
       <c r="B70" s="7">
         <f>sum(B56:B69)</f>
         <v>79</v>
       </c>
-      <c r="Q70" s="18"/>
+      <c r="Q70" s="21"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="Q71" s="18"/>
+      <c r="Q71" s="21"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q72" s="18"/>
+      <c r="A72" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q72" s="21"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="21" t="s">
-        <v>275</v>
-      </c>
-      <c r="B73" s="14">
+      <c r="A73" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="B73" s="13">
         <v>4.0</v>
       </c>
-      <c r="Q73" s="18"/>
+      <c r="Q73" s="21"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="21" t="s">
-        <v>276</v>
-      </c>
-      <c r="Q74" s="18"/>
+      <c r="A74" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q74" s="21"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="21" t="s">
-        <v>277</v>
-      </c>
-      <c r="B75" s="14">
+      <c r="A75" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="B75" s="13">
         <v>4.0</v>
       </c>
-      <c r="Q75" s="18"/>
+      <c r="Q75" s="21"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="B76" s="14">
+      <c r="A76" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="B76" s="13">
         <v>22.0</v>
       </c>
-      <c r="Q76" s="18"/>
+      <c r="Q76" s="21"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="B77" s="14">
+      <c r="A77" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="B77" s="13">
         <v>2.0</v>
       </c>
-      <c r="Q77" s="18"/>
+      <c r="Q77" s="21"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="14" t="s">
-        <v>274</v>
+      <c r="A78" s="13" t="s">
+        <v>280</v>
       </c>
       <c r="B78" s="7">
         <f>sum(B73:B77)</f>
         <v>32</v>
       </c>
-      <c r="Q78" s="18"/>
+      <c r="Q78" s="21"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="Q79" s="18"/>
+      <c r="Q79" s="21"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B80" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q80" s="18"/>
+      <c r="A80" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q80" s="21"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="21" t="s">
+      <c r="A81" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="B81" s="13">
+        <v>6.0</v>
+      </c>
+      <c r="Q81" s="21"/>
+    </row>
+    <row r="82" ht="15.75" customHeight="1">
+      <c r="A82" s="24" t="s">
+        <v>287</v>
+      </c>
+      <c r="B82" s="13">
+        <v>6.0</v>
+      </c>
+      <c r="Q82" s="21"/>
+    </row>
+    <row r="83" ht="15.75" customHeight="1">
+      <c r="A83" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="B83" s="13">
+        <v>6.0</v>
+      </c>
+      <c r="Q83" s="21"/>
+    </row>
+    <row r="84" ht="15.75" customHeight="1">
+      <c r="A84" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q84" s="21"/>
+    </row>
+    <row r="85" ht="15.75" customHeight="1">
+      <c r="A85" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q85" s="21"/>
+    </row>
+    <row r="86" ht="15.75" customHeight="1">
+      <c r="A86" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q86" s="21"/>
+    </row>
+    <row r="87" ht="15.75" customHeight="1">
+      <c r="A87" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="B87" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="Q87" s="21"/>
+    </row>
+    <row r="88" ht="15.75" customHeight="1">
+      <c r="A88" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="B88" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="Q88" s="21"/>
+    </row>
+    <row r="89" ht="15.75" customHeight="1">
+      <c r="A89" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="B89" s="13">
+        <v>20.0</v>
+      </c>
+      <c r="Q89" s="21"/>
+    </row>
+    <row r="90" ht="15.75" customHeight="1">
+      <c r="A90" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="B90" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="Q90" s="21"/>
+    </row>
+    <row r="91" ht="15.75" customHeight="1">
+      <c r="A91" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="B91" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="Q91" s="21"/>
+    </row>
+    <row r="92" ht="15.75" customHeight="1">
+      <c r="A92" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="B92" s="13">
+        <v>11.0</v>
+      </c>
+      <c r="Q92" s="21"/>
+    </row>
+    <row r="93" ht="15.75" customHeight="1">
+      <c r="A93" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="B93" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="Q93" s="21"/>
+    </row>
+    <row r="94" ht="15.75" customHeight="1">
+      <c r="A94" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="B94" s="13">
+        <v>5.0</v>
+      </c>
+      <c r="Q94" s="21"/>
+    </row>
+    <row r="95" ht="15.75" customHeight="1">
+      <c r="A95" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="B95" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="Q95" s="21"/>
+    </row>
+    <row r="96" ht="15.75" customHeight="1">
+      <c r="A96" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q96" s="21"/>
+    </row>
+    <row r="97" ht="15.75" customHeight="1">
+      <c r="A97" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="B97" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="Q97" s="21"/>
+    </row>
+    <row r="98" ht="15.75" customHeight="1">
+      <c r="A98" s="24" t="s">
+        <v>302</v>
+      </c>
+      <c r="B98" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="Q98" s="21"/>
+    </row>
+    <row r="99" ht="15.75" customHeight="1">
+      <c r="A99" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q99" s="21"/>
+    </row>
+    <row r="100" ht="15.75" customHeight="1">
+      <c r="A100" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="B100" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="Q100" s="21"/>
+    </row>
+    <row r="101" ht="15.75" customHeight="1">
+      <c r="A101" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="B101" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="Q101" s="21"/>
+    </row>
+    <row r="102" ht="15.75" customHeight="1">
+      <c r="A102" s="13" t="s">
         <v>280</v>
-      </c>
-      <c r="B81" s="14">
-        <v>6.0</v>
-      </c>
-      <c r="Q81" s="18"/>
-    </row>
-    <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="21" t="s">
-        <v>281</v>
-      </c>
-      <c r="B82" s="14">
-        <v>6.0</v>
-      </c>
-      <c r="Q82" s="18"/>
-    </row>
-    <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="B83" s="14">
-        <v>6.0</v>
-      </c>
-      <c r="Q83" s="18"/>
-    </row>
-    <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="21" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q84" s="18"/>
-    </row>
-    <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="21" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q85" s="18"/>
-    </row>
-    <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="21" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q86" s="18"/>
-    </row>
-    <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="21" t="s">
-        <v>285</v>
-      </c>
-      <c r="B87" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="Q87" s="18"/>
-    </row>
-    <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="21" t="s">
-        <v>286</v>
-      </c>
-      <c r="B88" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="Q88" s="18"/>
-    </row>
-    <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="21" t="s">
-        <v>287</v>
-      </c>
-      <c r="B89" s="14">
-        <v>20.0</v>
-      </c>
-      <c r="Q89" s="18"/>
-    </row>
-    <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="B90" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="Q90" s="18"/>
-    </row>
-    <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="21" t="s">
-        <v>289</v>
-      </c>
-      <c r="B91" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="Q91" s="18"/>
-    </row>
-    <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="B92" s="14">
-        <v>11.0</v>
-      </c>
-      <c r="Q92" s="18"/>
-    </row>
-    <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="B93" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="Q93" s="18"/>
-    </row>
-    <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="B94" s="14">
-        <v>5.0</v>
-      </c>
-      <c r="Q94" s="18"/>
-    </row>
-    <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="21" t="s">
-        <v>293</v>
-      </c>
-      <c r="B95" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="Q95" s="18"/>
-    </row>
-    <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="21" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q96" s="18"/>
-    </row>
-    <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="21" t="s">
-        <v>295</v>
-      </c>
-      <c r="B97" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="Q97" s="18"/>
-    </row>
-    <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="B98" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="Q98" s="18"/>
-    </row>
-    <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="21" t="s">
-        <v>297</v>
-      </c>
-      <c r="Q99" s="18"/>
-    </row>
-    <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="21" t="s">
-        <v>298</v>
-      </c>
-      <c r="B100" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="Q100" s="18"/>
-    </row>
-    <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="21" t="s">
-        <v>299</v>
-      </c>
-      <c r="B101" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="Q101" s="18"/>
-    </row>
-    <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="14" t="s">
-        <v>274</v>
       </c>
       <c r="B102" s="7">
         <f>sum(B81:B101)</f>
         <v>75</v>
       </c>
-      <c r="Q102" s="18"/>
+      <c r="Q102" s="21"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="Q103" s="18"/>
+      <c r="Q103" s="21"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="Q104" s="18"/>
+      <c r="Q104" s="21"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="Q105" s="18"/>
+      <c r="Q105" s="21"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="Q106" s="18"/>
+      <c r="Q106" s="21"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="Q107" s="18"/>
+      <c r="Q107" s="21"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="Q108" s="18"/>
+      <c r="Q108" s="21"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="Q109" s="18"/>
+      <c r="Q109" s="21"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="Q110" s="18"/>
+      <c r="Q110" s="21"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="Q111" s="18"/>
+      <c r="Q111" s="21"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="Q112" s="18"/>
+      <c r="Q112" s="21"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="Q113" s="18"/>
+      <c r="Q113" s="21"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="Q114" s="18"/>
+      <c r="Q114" s="21"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="Q115" s="18"/>
+      <c r="Q115" s="21"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="Q116" s="18"/>
+      <c r="Q116" s="21"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="Q117" s="18"/>
+      <c r="Q117" s="21"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="Q118" s="18"/>
+      <c r="Q118" s="21"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="Q119" s="18"/>
+      <c r="Q119" s="21"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="Q120" s="18"/>
+      <c r="Q120" s="21"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="Q121" s="18"/>
+      <c r="Q121" s="21"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="Q122" s="18"/>
+      <c r="Q122" s="21"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="Q123" s="18"/>
+      <c r="Q123" s="21"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="Q124" s="18"/>
+      <c r="Q124" s="21"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="Q125" s="18"/>
+      <c r="Q125" s="21"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="Q126" s="18"/>
+      <c r="Q126" s="21"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="Q127" s="18"/>
+      <c r="Q127" s="21"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="Q128" s="18"/>
+      <c r="Q128" s="21"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="Q129" s="18"/>
+      <c r="Q129" s="21"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="Q130" s="18"/>
+      <c r="Q130" s="21"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="Q131" s="18"/>
+      <c r="Q131" s="21"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="Q132" s="18"/>
+      <c r="Q132" s="21"/>
     </row>
     <row r="133" ht="15.75" customHeight="1"/>
     <row r="134" ht="15.75" customHeight="1"/>
@@ -6117,137 +6271,137 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>301</v>
-      </c>
-      <c r="D1" s="22"/>
+      <c r="A1" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="23">
+      <c r="A2" s="26">
         <v>1940.0</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="26">
         <v>539.0</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="23">
+      <c r="A3" s="26">
         <v>1941.0</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="26">
         <v>201.0</v>
       </c>
-      <c r="C3" s="24"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="23">
+      <c r="A4" s="26">
         <v>1942.0</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="26">
         <v>219.0</v>
       </c>
-      <c r="C4" s="24"/>
+      <c r="C4" s="27"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="23">
+      <c r="A5" s="26">
         <v>1943.0</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="26">
         <v>58.0</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="27"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="23">
+      <c r="A6" s="26">
         <v>1944.0</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="26">
         <v>66.0</v>
       </c>
-      <c r="C6" s="24"/>
+      <c r="C6" s="27"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="23">
+      <c r="A7" s="26">
         <v>1945.0</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="26">
         <v>239.0</v>
       </c>
-      <c r="C7" s="24"/>
+      <c r="C7" s="27"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="23">
+      <c r="A8" s="26">
         <v>1946.0</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="26">
         <v>140.0</v>
       </c>
-      <c r="C8" s="24"/>
+      <c r="C8" s="27"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="23">
+      <c r="A9" s="26">
         <v>1947.0</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="26">
         <v>292.0</v>
       </c>
-      <c r="C9" s="24"/>
+      <c r="C9" s="27"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="23">
+      <c r="A10" s="26">
         <v>1948.0</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="26">
         <v>394.0</v>
       </c>
-      <c r="C10" s="24"/>
+      <c r="C10" s="27"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="23">
+      <c r="A11" s="26">
         <v>1949.0</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B11" s="26">
         <v>149.0</v>
       </c>
-      <c r="C11" s="24"/>
+      <c r="C11" s="27"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="25" t="s">
-        <v>302</v>
+      <c r="A12" s="28" t="s">
+        <v>308</v>
       </c>
       <c r="B12" s="7">
         <f>sum(B2:B11)</f>
         <v>2297</v>
       </c>
-      <c r="C12" s="24"/>
+      <c r="C12" s="27"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="25" t="s">
-        <v>303</v>
-      </c>
-      <c r="C13" s="24"/>
+      <c r="A13" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="C13" s="27"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="25"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="24"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="14" t="s">
-        <v>304</v>
-      </c>
-      <c r="B15" s="14">
+      <c r="A15" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="B15" s="13">
         <v>521.0</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="14" t="s">
-        <v>305</v>
-      </c>
-      <c r="B16" s="26">
+      <c r="A16" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B16" s="29">
         <f>B15/B12</f>
         <v>0.2268175882</v>
       </c>
@@ -7262,145 +7416,145 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="27" t="s">
-        <v>306</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>307</v>
+      <c r="A1" s="30" t="s">
+        <v>312</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="28">
+      <c r="A2" s="31">
         <v>1940.0</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2" s="31">
         <v>512.0</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="31"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="28">
+      <c r="A3" s="31">
         <v>1941.0</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="31">
         <v>571.0</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="28">
+      <c r="A4" s="31">
         <v>1942.0</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="31">
         <v>421.0</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="31"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="28">
+      <c r="A5" s="31">
         <v>1943.0</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="31">
         <v>271.0</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="31"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="28">
+      <c r="A6" s="31">
         <v>1944.0</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="31">
         <v>16.0</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="31"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="28">
+      <c r="A7" s="31">
         <v>1945.0</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="31">
         <v>24.0</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="31"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="28">
+      <c r="A8" s="31">
         <v>1946.0</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="31">
         <v>81.0</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="31"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="28">
+      <c r="A9" s="31">
         <v>1947.0</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="31">
         <v>272.0</v>
       </c>
-      <c r="C9" s="28"/>
+      <c r="C9" s="31"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="28">
+      <c r="A10" s="31">
         <v>1948.0</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="31">
         <v>376.0</v>
       </c>
-      <c r="C10" s="28"/>
+      <c r="C10" s="31"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="28">
+      <c r="A11" s="31">
         <v>1949.0</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="31">
         <v>476.0</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="31"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="27" t="s">
-        <v>302</v>
-      </c>
-      <c r="B12" s="28">
+      <c r="A12" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="B12" s="31">
         <f>sum(B2:B11)</f>
         <v>3020</v>
       </c>
-      <c r="C12" s="28"/>
+      <c r="C12" s="31"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="27" t="s">
-        <v>308</v>
-      </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
+      <c r="A13" s="30" t="s">
+        <v>314</v>
+      </c>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="28" t="s">
-        <v>309</v>
-      </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
+      <c r="A14" s="31" t="s">
+        <v>315</v>
+      </c>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="27" t="s">
-        <v>310</v>
-      </c>
-      <c r="B15" s="27">
+      <c r="A15" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="B15" s="30">
         <v>190.0</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="31"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="27" t="s">
-        <v>311</v>
-      </c>
-      <c r="B16" s="29">
+      <c r="A16" s="30" t="s">
+        <v>317</v>
+      </c>
+      <c r="B16" s="32">
         <f>B15/B12</f>
         <v>0.06291390728</v>
       </c>
-      <c r="C16" s="28"/>
+      <c r="C16" s="31"/>
     </row>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>

</xml_diff>